<commit_message>
Atualização da Dashboard do Excel
Contexto dos Gráficos e atualização das KPIs
</commit_message>
<xml_diff>
--- a/Dashboard/DashBoard + KPIs.xlsx
+++ b/Dashboard/DashBoard + KPIs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/emmily_jesus_sptech_school/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9aaeaea6ef72b91c/Documentos/Repositórios de Projetos/Projeto_TechSolutions/Projeto-TechSolutions/Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1096" documentId="8_{79E0FDFA-817F-47F1-A30B-EBC0063B5569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{836B58FD-8753-412F-9567-ABF9C6D6E169}"/>
+  <xr:revisionPtr revIDLastSave="1139" documentId="8_{79E0FDFA-817F-47F1-A30B-EBC0063B5569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB70D954-6315-467D-9EB8-F59F297709B6}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{956D901D-5B0C-4BAE-8E2A-B98FFEB0B974}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{956D901D-5B0C-4BAE-8E2A-B98FFEB0B974}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
-  <si>
-    <t>SENSORES</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>KPIs</t>
-  </si>
-  <si>
-    <t>Sensor 1</t>
-  </si>
-  <si>
-    <t>Sensor 2</t>
   </si>
   <si>
     <t>Umidade</t>
@@ -60,9 +51,6 @@
   </si>
   <si>
     <t>Umidade_Média</t>
-  </si>
-  <si>
-    <t>SENSOR 1</t>
   </si>
   <si>
     <t>Alertas</t>
@@ -79,12 +67,21 @@
   <si>
     <t>Vermelho</t>
   </si>
+  <si>
+    <t>Armazens</t>
+  </si>
+  <si>
+    <t>Armazem 1</t>
+  </si>
+  <si>
+    <t>Armazem 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -324,12 +321,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,6 +328,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -396,8 +390,21 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Sensores</a:t>
+              <a:rPr lang="en-US" sz="1300" b="1"/>
+              <a:t>Média</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1300" b="1" baseline="0"/>
+              <a:t> por hora da umidade por armazém de café </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1300" b="1" baseline="0"/>
+              <a:t>no dia 20.10.23</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -426,7 +433,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -441,11 +448,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$G$4</c:f>
+              <c:f>Dashboard!$H$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sensor 1</c:v>
+                  <c:v>Armazem 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -470,7 +477,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Dashboard!$F$6:$F$15</c:f>
+              <c:f>Dashboard!$G$6:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>h:mm</c:formatCode>
                 <c:ptCount val="10"/>
@@ -509,7 +516,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$G$6:$G$15</c:f>
+              <c:f>Dashboard!$H$6:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -558,11 +565,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$H$4</c:f>
+              <c:f>Dashboard!$I$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sensor 2</c:v>
+                  <c:v>Armazem 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -587,7 +594,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Dashboard!$F$6:$F$15</c:f>
+              <c:f>Dashboard!$G$6:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>h:mm</c:formatCode>
                 <c:ptCount val="10"/>
@@ -626,7 +633,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$H$6:$H$15</c:f>
+              <c:f>Dashboard!$I$6:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -771,7 +778,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -802,7 +809,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="763521088"/>
@@ -894,7 +901,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -925,7 +932,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="752716832"/>
@@ -966,7 +973,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1006,7 +1013,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1037,12 +1044,64 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
               <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
+                  <a:sysClr val="window" lastClr="FFFFFF">
                     <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF">
+                    <a:lumMod val="85000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Média por hora da umidade por armazém de café </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF">
+                    <a:lumMod val="85000"/>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1051,7 +1110,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sensores</a:t>
+              <a:t>no dia 20.10.23</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1068,19 +1127,33 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
+                <a:sysClr val="window" lastClr="FFFFFF">
                   <a:lumMod val="85000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1096,11 +1169,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$G$4</c:f>
+              <c:f>Dashboard!$H$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sensor 1</c:v>
+                  <c:v>Armazem 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1149,7 +1222,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1181,7 +1254,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Dashboard!$F$6:$F$15</c:f>
+              <c:f>Dashboard!$G$6:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>h:mm</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1220,7 +1293,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$G$6:$G$15</c:f>
+              <c:f>Dashboard!$H$6:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1268,11 +1341,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$H$4</c:f>
+              <c:f>Dashboard!$I$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sensor 2</c:v>
+                  <c:v>Armazem 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1321,7 +1394,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1353,7 +1426,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Dashboard!$F$6:$F$15</c:f>
+              <c:f>Dashboard!$G$6:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>h:mm</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1392,7 +1465,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$H$6:$H$15</c:f>
+              <c:f>Dashboard!$I$6:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1538,7 +1611,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1569,7 +1642,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="763521088"/>
@@ -1661,7 +1734,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1692,7 +1765,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="752716832"/>
@@ -1733,7 +1806,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1773,7 +1846,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1830,7 +1903,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1844,7 +1917,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$T$11</c:f>
+              <c:f>Dashboard!$U$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1973,7 +2046,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="bestFit"/>
@@ -2003,7 +2076,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Dashboard!$T$12:$T$15</c:f>
+              <c:f>Dashboard!$U$12:$U$15</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2023,7 +2096,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$U$12:$U$15</c:f>
+              <c:f>Dashboard!$V$12:$V$15</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2094,7 +2167,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2142,7 +2215,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2192,7 +2265,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2207,11 +2280,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$AC$8</c:f>
+              <c:f>Dashboard!$AD$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SENSOR 1</c:v>
+                  <c:v>Armazem 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2280,7 +2353,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -2312,7 +2385,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Dashboard!$AC$10:$AC$15</c:f>
+              <c:f>Dashboard!$AD$10:$AD$15</c:f>
               <c:numCache>
                 <c:formatCode>h:mm</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2339,7 +2412,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$AD$10:$AD$15</c:f>
+              <c:f>Dashboard!$AE$10:$AE$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2444,7 +2517,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="747597584"/>
@@ -2514,7 +2587,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="592318928"/>
@@ -2565,7 +2638,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4889,7 +4962,7 @@
       <xdr:rowOff>166352</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>969435</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>964</xdr:rowOff>
@@ -4919,13 +4992,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>125074</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>9621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>529167</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>25208</xdr:rowOff>
@@ -4957,13 +5030,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>352726</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>178557</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>14059</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>37949</xdr:rowOff>
@@ -4996,13 +5069,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>73045</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>41650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>458463</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>156502</xdr:rowOff>
@@ -5034,7 +5107,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5330,328 +5403,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46222F9F-7533-433A-A1A2-C80AE37F247D}">
-  <dimension ref="B3:AD19"/>
+  <dimension ref="B3:AE19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="8" width="20.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="19" max="19" width="7.140625" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" customWidth="1"/>
-    <col min="21" max="21" width="12.85546875" customWidth="1"/>
-    <col min="29" max="29" width="11.5703125" customWidth="1"/>
-    <col min="30" max="30" width="12" customWidth="1"/>
-    <col min="31" max="32" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="20" max="20" width="7.109375" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" customWidth="1"/>
+    <col min="22" max="22" width="12.88671875" customWidth="1"/>
+    <col min="30" max="30" width="11.5546875" customWidth="1"/>
+    <col min="31" max="31" width="12" customWidth="1"/>
+    <col min="32" max="33" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:30" ht="18">
-      <c r="F3" s="18" t="s">
+    <row r="3" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="C3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
+      <c r="G3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="2:30" ht="18">
-      <c r="B4" s="21" t="s">
+    <row r="4" spans="2:31" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14" t="s">
+      <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:30" ht="15.6">
-      <c r="B5" s="6" t="s">
+      <c r="H5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="P5" s="1"/>
+      <c r="I5" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="X5" s="1"/>
+      <c r="T5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="2:30" ht="15.6">
+    <row r="6" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
         <v>100</v>
       </c>
-      <c r="C6" s="15">
+      <c r="D6" s="15">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F6" s="16">
+      <c r="G6" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G6" s="12">
+      <c r="H6" s="12">
         <v>95</v>
       </c>
-      <c r="H6" s="12">
+      <c r="I6" s="12">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="2:30" ht="15.6">
+    <row r="7" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="13">
         <v>90</v>
       </c>
-      <c r="C7" s="15">
+      <c r="D7" s="15">
         <v>0.45833333333333331</v>
       </c>
-      <c r="F7" s="16">
+      <c r="G7" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G7" s="12">
+      <c r="H7" s="12">
         <v>66</v>
       </c>
-      <c r="H7" s="12">
+      <c r="I7" s="12">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:30" ht="15.6">
+    <row r="8" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
         <v>80</v>
       </c>
-      <c r="C8" s="15">
+      <c r="D8" s="15">
         <v>0.5</v>
       </c>
-      <c r="F8" s="16">
+      <c r="G8" s="16">
         <v>0.5</v>
       </c>
-      <c r="G8" s="12">
+      <c r="H8" s="12">
         <v>59</v>
       </c>
-      <c r="H8" s="12">
+      <c r="I8" s="12">
         <v>80</v>
       </c>
-      <c r="AC8" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD8" s="24"/>
+      <c r="AD8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE8" s="22"/>
     </row>
-    <row r="9" spans="2:30" ht="15.6">
+    <row r="9" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
         <v>70</v>
       </c>
-      <c r="C9" s="15">
+      <c r="D9" s="15">
         <v>0.54166666666666696</v>
       </c>
-      <c r="F9" s="16">
+      <c r="G9" s="16">
         <v>0.54166666666666696</v>
       </c>
-      <c r="G9" s="12">
+      <c r="H9" s="12">
         <v>70</v>
       </c>
-      <c r="H9" s="12">
+      <c r="I9" s="12">
         <v>44</v>
       </c>
-      <c r="AC9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>4</v>
+      <c r="AD9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:30" ht="15.6">
+    <row r="10" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
         <v>60</v>
       </c>
-      <c r="C10" s="15">
+      <c r="D10" s="15">
         <v>0.58333333333333304</v>
       </c>
-      <c r="F10" s="16">
+      <c r="G10" s="16">
         <v>0.58333333333333304</v>
       </c>
-      <c r="G10" s="12">
+      <c r="H10" s="12">
         <v>25</v>
       </c>
-      <c r="H10" s="12">
+      <c r="I10" s="12">
         <v>66</v>
       </c>
-      <c r="AC10" s="2">
+      <c r="AD10" s="2">
         <v>0.4236111111111111</v>
       </c>
-      <c r="AD10" s="3">
+      <c r="AE10" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="2:30" ht="18">
+    <row r="11" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B11" s="13">
         <v>50</v>
       </c>
-      <c r="C11" s="15">
+      <c r="D11" s="15">
         <v>0.625</v>
       </c>
-      <c r="F11" s="16">
+      <c r="G11" s="16">
         <v>0.625</v>
       </c>
-      <c r="G11" s="12">
+      <c r="H11" s="12">
         <v>89</v>
       </c>
-      <c r="H11" s="12">
+      <c r="I11" s="12">
         <v>63</v>
       </c>
-      <c r="T11" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="U11" s="25"/>
-      <c r="AC11" s="2">
+      <c r="U11" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="V11" s="23"/>
+      <c r="AD11" s="2">
         <v>0.43055555555555558</v>
       </c>
-      <c r="AD11" s="3">
+      <c r="AE11" s="3">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="2:30" ht="15.6">
+    <row r="12" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
         <v>40</v>
       </c>
-      <c r="C12" s="15">
+      <c r="D12" s="15">
         <v>0.66666666666666696</v>
       </c>
-      <c r="F12" s="16">
+      <c r="G12" s="16">
         <v>0.66666666666666696</v>
       </c>
-      <c r="G12" s="12">
+      <c r="H12" s="12">
         <v>61</v>
       </c>
-      <c r="H12" s="12">
+      <c r="I12" s="12">
         <v>20</v>
       </c>
-      <c r="T12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="U12" s="9">
+      <c r="U12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="V12" s="9">
         <v>0.2</v>
       </c>
-      <c r="AC12" s="2">
+      <c r="AD12" s="2">
         <v>0.4375</v>
       </c>
-      <c r="AD12" s="3">
+      <c r="AE12" s="3">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="2:30" ht="15.6">
+    <row r="13" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="13">
         <v>30</v>
       </c>
-      <c r="C13" s="15">
+      <c r="D13" s="15">
         <v>0.70833333333333304</v>
       </c>
-      <c r="F13" s="16">
+      <c r="G13" s="16">
         <v>0.70833333333333304</v>
       </c>
-      <c r="G13" s="12">
+      <c r="H13" s="12">
         <v>63</v>
       </c>
-      <c r="H13" s="12">
+      <c r="I13" s="12">
         <v>60</v>
       </c>
-      <c r="T13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="U13" s="9">
+      <c r="U13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="V13" s="9">
         <v>0.2</v>
       </c>
-      <c r="AC13" s="2">
+      <c r="AD13" s="2">
         <v>0.44444444444444497</v>
       </c>
-      <c r="AD13" s="3">
+      <c r="AE13" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="2:30" ht="15.6">
+    <row r="14" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="13">
         <v>20</v>
       </c>
-      <c r="C14" s="15">
+      <c r="D14" s="15">
         <v>0.75</v>
       </c>
-      <c r="F14" s="16">
+      <c r="G14" s="16">
         <v>0.75</v>
       </c>
-      <c r="G14" s="12">
+      <c r="H14" s="12">
         <v>30</v>
       </c>
-      <c r="H14" s="12">
+      <c r="I14" s="12">
         <v>72</v>
       </c>
-      <c r="T14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="U14" s="9">
+      <c r="U14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="V14" s="9">
         <v>0.45</v>
       </c>
-      <c r="AC14" s="2">
+      <c r="AD14" s="2">
         <v>0.45138888888888901</v>
       </c>
-      <c r="AD14" s="3">
+      <c r="AE14" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:30" ht="15.6">
+    <row r="15" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="13">
         <v>10</v>
       </c>
-      <c r="C15" s="15">
+      <c r="D15" s="15">
         <v>0.79166666666666696</v>
       </c>
-      <c r="F15" s="16">
+      <c r="G15" s="16">
         <v>0.79166666666666696</v>
       </c>
-      <c r="G15" s="12">
+      <c r="H15" s="12">
         <v>66</v>
       </c>
-      <c r="H15" s="12">
+      <c r="I15" s="12">
         <v>80</v>
       </c>
-      <c r="T15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="U15" s="9">
+      <c r="U15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="V15" s="9">
         <v>0.15</v>
       </c>
-      <c r="AC15" s="2">
+      <c r="AD15" s="2">
         <v>0.45833333333333298</v>
       </c>
-      <c r="AD15" s="3">
+      <c r="AE15" s="3">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="6:6" ht="15">
-      <c r="F19" s="17"/>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G19" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="T11:U11"/>
+  <mergeCells count="3">
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="U11:V11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>